<commit_message>
update excel files and table header
</commit_message>
<xml_diff>
--- a/public/bandwidth_customers.xlsx
+++ b/public/bandwidth_customers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaree\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EAC3E8-742A-4A09-B095-A3833F151F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA43A0D2-2116-4BA5-B8AE-59C3A548C891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8564000C-5963-4787-840A-8A97EBE72C31}"/>
   </bookViews>
@@ -138,7 +138,7 @@
     <t>Last modified by</t>
   </si>
   <si>
-    <t>Created date &amp; time</t>
+    <t>Last modified date &amp; time</t>
   </si>
 </sst>
 </file>

</xml_diff>